<commit_message>
started working on a process to get pivot tables to generate with xlwings. It's not quite working.
</commit_message>
<xml_diff>
--- a/Workbooks/pivot_table_example.xlsx
+++ b/Workbooks/pivot_table_example.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tjinspection2-my.sharepoint.com/personal/nicholas_licalsi_tjinspection_net/Documents/Documents/Code/xlwings_testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlicalsi\Documents\Code\xlwings_testing\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{351A9840-71E3-4123-A59C-1B0BF2229365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF955B32-1078-4F92-ADE6-084A7C89AEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4CC8B600-BEAC-4E55-90F1-5561AC102CE2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4CC8B600-BEAC-4E55-90F1-5561AC102CE2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Pivot" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,9 +36,105 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Doll</t>
+  </si>
+  <si>
+    <t>Toy</t>
+  </si>
+  <si>
+    <t>A doll to play with</t>
+  </si>
+  <si>
+    <t>Cards</t>
+  </si>
+  <si>
+    <t>A card game to play</t>
+  </si>
+  <si>
+    <t>Carrot</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>A carrot to eat</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t>An onion to eat</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>A flat screen tv</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>A computer to use</t>
+  </si>
+  <si>
+    <t>Sandwich</t>
+  </si>
+  <si>
+    <t>A sandwich to eat</t>
+  </si>
+  <si>
+    <t>Soda</t>
+  </si>
+  <si>
+    <t>Drink</t>
+  </si>
+  <si>
+    <t>A soda to drink</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +160,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -83,6 +183,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3AD56968-B6EE-493B-BD77-3D8937E172B7}" name="Table1" displayName="Table1" ref="A1:F9" totalsRowShown="0">
+  <autoFilter ref="A1:F9" xr:uid="{3AD56968-B6EE-493B-BD77-3D8937E172B7}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{5CC95AB3-33AE-423C-99A1-12D62CFD79E2}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{7432E7E1-3870-4797-AA37-6F944986AEE0}" name="Category"/>
+    <tableColumn id="3" xr3:uid="{5EDDBC9F-EDCC-4F71-8D47-271AC84EEE85}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{B261EA35-F3AA-4C32-AD26-59893422993B}" name="Price" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{8A69CB29-4790-4C93-BA4A-53DF7F5762D5}" name="Qty"/>
+    <tableColumn id="6" xr3:uid="{EC4331AD-225B-4AA8-9722-5C3D4733CADE}" name="Total" dataCellStyle="Currency">
+      <calculatedColumnFormula>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,12 +518,226 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A38F48-A100-4EB8-AA11-867F74A1A63F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9DC463-3110-4A6B-A95A-345D35894B16}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1100</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF3ACA-F3CC-405F-B7F0-3A5E8D6A538D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
got the pivot table example working
</commit_message>
<xml_diff>
--- a/Workbooks/pivot_table_example.xlsx
+++ b/Workbooks/pivot_table_example.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlicalsi\Documents\Code\xlwings_testing\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF955B32-1078-4F92-ADE6-084A7C89AEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F536F9DB-1278-409A-9159-019E9E7F25A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4CC8B600-BEAC-4E55-90F1-5561AC102CE2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4CC8B600-BEAC-4E55-90F1-5561AC102CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Pivot" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -118,6 +121,33 @@
   </si>
   <si>
     <t>A soda to drink</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Name</t>
+  </si>
+  <si>
+    <t>Sum of Qty</t>
+  </si>
+  <si>
+    <t>Sum of Total</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Jill</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
+    <t>Jo</t>
   </si>
 </sst>
 </file>
@@ -164,9 +194,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -185,11 +219,194 @@
 </styleSheet>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nicholas Licalsi" refreshedDate="46040.346471874996" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="8" xr:uid="{BC9B8326-A7AC-4CBB-AE81-46A431593F8A}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:G9" sheet="Sheet2"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Name" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Category" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Toy"/>
+        <s v="Game"/>
+        <s v="Food"/>
+        <s v="Technology"/>
+        <s v="Drink"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Description" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Price" numFmtId="44">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="1100"/>
+    </cacheField>
+    <cacheField name="Qty" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="10"/>
+    </cacheField>
+    <cacheField name="Total" numFmtId="44">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="3" maxValue="2000"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="8">
+  <r>
+    <s v="Doll"/>
+    <x v="0"/>
+    <s v="A doll to play with"/>
+    <n v="10"/>
+    <n v="2"/>
+    <n v="20"/>
+  </r>
+  <r>
+    <s v="Cards"/>
+    <x v="1"/>
+    <s v="A card game to play"/>
+    <n v="5"/>
+    <n v="10"/>
+    <n v="50"/>
+  </r>
+  <r>
+    <s v="Carrot"/>
+    <x v="2"/>
+    <s v="A carrot to eat"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Onion"/>
+    <x v="2"/>
+    <s v="An onion to eat"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="TV"/>
+    <x v="3"/>
+    <s v="A flat screen tv"/>
+    <n v="1100"/>
+    <n v="1"/>
+    <n v="1100"/>
+  </r>
+  <r>
+    <s v="Computer"/>
+    <x v="3"/>
+    <s v="A computer to use"/>
+    <n v="1000"/>
+    <n v="2"/>
+    <n v="2000"/>
+  </r>
+  <r>
+    <s v="Sandwich"/>
+    <x v="2"/>
+    <s v="A sandwich to eat"/>
+    <n v="10"/>
+    <n v="3"/>
+    <n v="30"/>
+  </r>
+  <r>
+    <s v="Soda"/>
+    <x v="4"/>
+    <s v="A soda to drink"/>
+    <n v="7"/>
+    <n v="3"/>
+    <n v="21"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{324926FF-B62E-4A9F-9495-4C16B85FC912}" name="PT_All_Rows" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="44" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Count of Name" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Qty" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="1" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3AD56968-B6EE-493B-BD77-3D8937E172B7}" name="Table1" displayName="Table1" ref="A1:F9" totalsRowShown="0">
-  <autoFilter ref="A1:F9" xr:uid="{3AD56968-B6EE-493B-BD77-3D8937E172B7}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3AD56968-B6EE-493B-BD77-3D8937E172B7}" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0">
+  <autoFilter ref="A1:G9" xr:uid="{3AD56968-B6EE-493B-BD77-3D8937E172B7}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{5CC95AB3-33AE-423C-99A1-12D62CFD79E2}" name="Name"/>
+    <tableColumn id="7" xr3:uid="{9E896EDF-68A6-4406-B1DC-48179D7F6F30}" name="Customer"/>
     <tableColumn id="2" xr3:uid="{7432E7E1-3870-4797-AA37-6F944986AEE0}" name="Category"/>
     <tableColumn id="3" xr3:uid="{5EDDBC9F-EDCC-4F71-8D47-271AC84EEE85}" name="Description"/>
     <tableColumn id="4" xr3:uid="{B261EA35-F3AA-4C32-AD26-59893422993B}" name="Price" dataCellStyle="Currency"/>
@@ -519,204 +736,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9DC463-3110-4A6B-A95A-345D35894B16}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>1100</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
         <v>1100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>1000</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>10</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>3</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>7</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>3</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Price]]</f>
         <v>21</v>
       </c>
@@ -731,14 +978,119 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF3ACA-F3CC-405F-B7F0-3A5E8D6A538D}">
-  <dimension ref="A1"/>
+  <dimension ref="A3:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3228</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added an outer and inner grouping
</commit_message>
<xml_diff>
--- a/Workbooks/pivot_table_example.xlsx
+++ b/Workbooks/pivot_table_example.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlicalsi\Documents\Code\xlwings_testing\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F536F9DB-1278-409A-9159-019E9E7F25A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4B508D-7F01-4036-9727-92AF47A56019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4CC8B600-BEAC-4E55-90F1-5561AC102CE2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Pivot" sheetId="3" r:id="rId2"/>
+    <sheet name="Pivot" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -194,12 +194,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -220,13 +223,20 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nicholas Licalsi" refreshedDate="46040.346471874996" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="8" xr:uid="{BC9B8326-A7AC-4CBB-AE81-46A431593F8A}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nicholas Licalsi" refreshedDate="46040.349374768521" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="8" xr:uid="{946A866F-CB17-4CE2-82CD-9D7B9854AD4A}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G9" sheet="Sheet2"/>
   </cacheSource>
-  <cacheFields count="6">
+  <cacheFields count="7">
     <cacheField name="Name" numFmtId="0">
       <sharedItems/>
+    </cacheField>
+    <cacheField name="Customer" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Jill"/>
+        <s v="Jim"/>
+        <s v="Jo"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Category" numFmtId="0">
       <sharedItems count="5">
@@ -263,6 +273,7 @@
   <r>
     <s v="Doll"/>
     <x v="0"/>
+    <x v="0"/>
     <s v="A doll to play with"/>
     <n v="10"/>
     <n v="2"/>
@@ -270,6 +281,7 @@
   </r>
   <r>
     <s v="Cards"/>
+    <x v="1"/>
     <x v="1"/>
     <s v="A card game to play"/>
     <n v="5"/>
@@ -279,6 +291,7 @@
   <r>
     <s v="Carrot"/>
     <x v="2"/>
+    <x v="2"/>
     <s v="A carrot to eat"/>
     <n v="2"/>
     <n v="2"/>
@@ -287,6 +300,7 @@
   <r>
     <s v="Onion"/>
     <x v="2"/>
+    <x v="2"/>
     <s v="An onion to eat"/>
     <n v="1"/>
     <n v="3"/>
@@ -294,6 +308,7 @@
   </r>
   <r>
     <s v="TV"/>
+    <x v="1"/>
     <x v="3"/>
     <s v="A flat screen tv"/>
     <n v="1100"/>
@@ -302,6 +317,7 @@
   </r>
   <r>
     <s v="Computer"/>
+    <x v="1"/>
     <x v="3"/>
     <s v="A computer to use"/>
     <n v="1000"/>
@@ -310,6 +326,7 @@
   </r>
   <r>
     <s v="Sandwich"/>
+    <x v="0"/>
     <x v="2"/>
     <s v="A sandwich to eat"/>
     <n v="10"/>
@@ -318,6 +335,7 @@
   </r>
   <r>
     <s v="Soda"/>
+    <x v="2"/>
     <x v="4"/>
     <s v="A soda to drink"/>
     <n v="7"/>
@@ -328,10 +346,18 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{324926FF-B62E-4A9F-9495-4C16B85FC912}" name="PT_All_Rows" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:D9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E42A5EB4-59EB-492E-9388-034625662785}" name="PT_All_Rows" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="6">
         <item x="4"/>
@@ -347,24 +373,37 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" numFmtId="44" showAll="0"/>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
     <field x="1"/>
+    <field x="2"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="10">
     <i>
       <x/>
     </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
     <i>
       <x v="1"/>
     </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
     <i>
       <x v="2"/>
     </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -386,8 +425,8 @@
   </colItems>
   <dataFields count="3">
     <dataField name="Count of Name" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Qty" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Qty" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="1" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -735,10 +774,185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF3ACA-F3CC-405F-B7F0-3A5E8D6A538D}">
+  <dimension ref="A3:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>26</v>
+      </c>
+      <c r="D13">
+        <v>3228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9DC463-3110-4A6B-A95A-345D35894B16}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -974,123 +1188,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF3ACA-F3CC-405F-B7F0-3A5E8D6A538D}">
-  <dimension ref="A3:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1">
-        <v>3100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3228</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
made a pivot builder object and wrapper
</commit_message>
<xml_diff>
--- a/Workbooks/pivot_table_example.xlsx
+++ b/Workbooks/pivot_table_example.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlicalsi\Documents\Code\xlwings_testing\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4B508D-7F01-4036-9727-92AF47A56019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0471BC-ADD3-45D3-9B34-0683CE546408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4CC8B600-BEAC-4E55-90F1-5561AC102CE2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4CC8B600-BEAC-4E55-90F1-5561AC102CE2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pivot" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Pivot" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -123,39 +123,40 @@
     <t>A soda to drink</t>
   </si>
   <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Jill</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
+    <t>Jo</t>
+  </si>
+  <si>
     <t>Row Labels</t>
   </si>
   <si>
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Count of Name</t>
-  </si>
-  <si>
-    <t>Sum of Qty</t>
-  </si>
-  <si>
-    <t>Sum of Total</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Jill</t>
-  </si>
-  <si>
-    <t>Jim</t>
-  </si>
-  <si>
-    <t>Jo</t>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>Total Qty</t>
+  </si>
+  <si>
+    <t>Total Spent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -194,7 +195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -204,6 +205,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -223,7 +226,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nicholas Licalsi" refreshedDate="46040.349374768521" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="8" xr:uid="{946A866F-CB17-4CE2-82CD-9D7B9854AD4A}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nicholas Licalsi" refreshedDate="46040.390743171294" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="8" xr:uid="{F1B931C3-461C-4C7B-80B3-266D5B999E7E}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G9" sheet="Sheet2"/>
   </cacheSource>
@@ -346,7 +349,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E42A5EB4-59EB-492E-9388-034625662785}" name="PT_All_Rows" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{509891DC-99C7-407C-9F59-823C6A590A2D}" name="PT_By_Customer" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -424,9 +427,9 @@
     </i>
   </colItems>
   <dataFields count="3">
-    <dataField name="Count of Name" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Qty" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Orders" fld="0" subtotal="count" baseField="0" baseItem="0" numFmtId="1"/>
+    <dataField name="Total Qty" fld="5" baseField="0" baseItem="0" numFmtId="1"/>
+    <dataField name="Total Spent" fld="6" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="1" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -774,181 +777,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF3ACA-F3CC-405F-B7F0-3A5E8D6A538D}">
-  <dimension ref="A3:D13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>3150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>3100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="C13">
-        <v>26</v>
-      </c>
-      <c r="D13">
-        <v>3228</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9DC463-3110-4A6B-A95A-345D35894B16}">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -972,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -995,7 +823,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1019,7 +847,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1043,7 +871,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1067,7 +895,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1091,7 +919,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -1115,7 +943,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -1139,7 +967,7 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -1163,7 +991,7 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -1188,4 +1016,177 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DADD068-DB30-4F19-A716-9E0FB456EB07}">
+  <dimension ref="A3:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+      <c r="C9" s="5">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="5">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5">
+        <v>3</v>
+      </c>
+      <c r="D11" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="5">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5">
+        <v>26</v>
+      </c>
+      <c r="D13" s="6">
+        <v>3228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cleaned up some of the naming conventions
</commit_message>
<xml_diff>
--- a/Workbooks/pivot_table_example.xlsx
+++ b/Workbooks/pivot_table_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlicalsi\Documents\Code\xlwings_testing\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0471BC-ADD3-45D3-9B34-0683CE546408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F643AB-3A3C-47DA-A641-799A958DDB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4CC8B600-BEAC-4E55-90F1-5561AC102CE2}"/>
   </bookViews>
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nicholas Licalsi" refreshedDate="46040.390743171294" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="8" xr:uid="{F1B931C3-461C-4C7B-80B3-266D5B999E7E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nicholas Licalsi" refreshedDate="46040.39780810185" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="8" xr:uid="{AD74BF40-A3A8-4A15-8A27-11C7F5E979AD}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G9" sheet="Sheet2"/>
   </cacheSource>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{509891DC-99C7-407C-9F59-823C6A590A2D}" name="PT_By_Customer" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3974AC91-5B29-42D7-BB5B-9A9CD81F5DAC}" name="PT_By_Customer" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -1019,7 +1019,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DADD068-DB30-4F19-A716-9E0FB456EB07}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066979C3-3D7B-4C3B-B195-A77C1642C8AB}">
   <dimension ref="A3:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>